<commit_message>
Kmeans done, working on kspecial
</commit_message>
<xml_diff>
--- a/cbir/doc/kspecialclassifier.xlsx
+++ b/cbir/doc/kspecialclassifier.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="108" windowWidth="15120" windowHeight="8016" activeTab="3"/>
+    <workbookView xWindow="120" yWindow="108" windowWidth="15120" windowHeight="8016" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="K-Optimierung" sheetId="1" r:id="rId1"/>
     <sheet name="Min-Class-Size" sheetId="2" r:id="rId2"/>
     <sheet name="size" sheetId="3" r:id="rId3"/>
     <sheet name="K-Means-op" sheetId="4" r:id="rId4"/>
+    <sheet name="resultat" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="18">
   <si>
     <t>K100</t>
   </si>
@@ -68,6 +69,9 @@
   </si>
   <si>
     <t>20 Iterations</t>
+  </si>
+  <si>
+    <t>resultat</t>
   </si>
 </sst>
 </file>
@@ -409,7 +413,7 @@
   <dimension ref="D1:R15"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:H15"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -1175,7 +1179,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="D13" sqref="D13:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -1468,20 +1472,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -1490,6 +1494,321 @@
       </c>
       <c r="G2" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="D3">
+        <v>96.078431372549005</v>
+      </c>
+      <c r="E3">
+        <v>728.40372792311996</v>
+      </c>
+      <c r="G3">
+        <v>84.313725490196006</v>
+      </c>
+      <c r="H3">
+        <v>795.480678201091</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="D4">
+        <v>90.196078431372499</v>
+      </c>
+      <c r="E4">
+        <v>799.32365556956699</v>
+      </c>
+      <c r="G4">
+        <v>88.235294117647001</v>
+      </c>
+      <c r="H4">
+        <v>792.93568962689403</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="D5">
+        <v>90.196078431372499</v>
+      </c>
+      <c r="E5">
+        <v>828.21145603015998</v>
+      </c>
+      <c r="G5">
+        <v>92.156862745097996</v>
+      </c>
+      <c r="H5">
+        <v>819.98763359585303</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="D6">
+        <v>92.156862745097996</v>
+      </c>
+      <c r="E6">
+        <v>780.70901257657601</v>
+      </c>
+      <c r="G6">
+        <v>88.235294117647001</v>
+      </c>
+      <c r="H6">
+        <v>830.71503483404297</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="D7">
+        <v>88.235294117647001</v>
+      </c>
+      <c r="E7">
+        <v>812.28013661959596</v>
+      </c>
+      <c r="G7">
+        <v>88.235294117647001</v>
+      </c>
+      <c r="H7">
+        <v>830.50790859531605</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="D8">
+        <v>72.549019607843107</v>
+      </c>
+      <c r="E8">
+        <v>757.41424743066705</v>
+      </c>
+      <c r="G8">
+        <v>92.156862745097996</v>
+      </c>
+      <c r="H8">
+        <v>754.11172204172601</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="D9">
+        <v>80.392156862745097</v>
+      </c>
+      <c r="E9">
+        <v>792.672391214546</v>
+      </c>
+      <c r="G9">
+        <v>74.509803921568604</v>
+      </c>
+      <c r="H9">
+        <v>837.07231558155695</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="D10">
+        <v>76.470588235294102</v>
+      </c>
+      <c r="E10">
+        <v>796.07376248407604</v>
+      </c>
+      <c r="G10">
+        <v>88.235294117647001</v>
+      </c>
+      <c r="H10">
+        <v>865.87959394217103</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="D11">
+        <v>80.392156862745097</v>
+      </c>
+      <c r="E11">
+        <v>831.14813299214097</v>
+      </c>
+      <c r="G11">
+        <v>88.235294117647001</v>
+      </c>
+      <c r="H11">
+        <v>779.25624386648599</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="D12">
+        <v>92.156862745097996</v>
+      </c>
+      <c r="E12">
+        <v>812.54875971218996</v>
+      </c>
+      <c r="G12">
+        <v>92.156862745097996</v>
+      </c>
+      <c r="H12">
+        <v>724.06236605660501</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="D14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14">
+        <f>MIN(E3:E12)</f>
+        <v>728.40372792311996</v>
+      </c>
+      <c r="G14" t="s">
+        <v>3</v>
+      </c>
+      <c r="H14">
+        <f>MIN(H3:H12)</f>
+        <v>724.06236605660501</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="D15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15">
+        <f>MAX(E3:E12)</f>
+        <v>831.14813299214097</v>
+      </c>
+      <c r="G15" t="s">
+        <v>4</v>
+      </c>
+      <c r="H15">
+        <f>MAX(H3:H12)</f>
+        <v>865.87959394217103</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="D16" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16">
+        <f>AVERAGE(E3:E12)</f>
+        <v>793.87852825526386</v>
+      </c>
+      <c r="G16" t="s">
+        <v>5</v>
+      </c>
+      <c r="H16">
+        <f>AVERAGE(H3:H12)</f>
+        <v>803.00091863417424</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>88.235294117647001</v>
+      </c>
+      <c r="B2">
+        <v>775.261286845364</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>84.313725490196006</v>
+      </c>
+      <c r="B3">
+        <v>909.30577135828798</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>91.176470588235205</v>
+      </c>
+      <c r="B4">
+        <v>781.51136223044</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>84.313725490196006</v>
+      </c>
+      <c r="B5">
+        <v>745.01071609957501</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>92.156862745097996</v>
+      </c>
+      <c r="B6">
+        <v>666.24564536347998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>88.235294117647001</v>
+      </c>
+      <c r="B7">
+        <v>710.91349814873297</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8">
+        <v>92.156862745097996</v>
+      </c>
+      <c r="B8">
+        <v>675.896966549784</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9">
+        <v>84.313725490196006</v>
+      </c>
+      <c r="B9">
+        <v>704.743628750163</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
+        <v>92.156862745097996</v>
+      </c>
+      <c r="B10">
+        <v>798.27858756595197</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11">
+        <v>78.431372549019599</v>
+      </c>
+      <c r="B11">
+        <v>766.75048645495303</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13">
+        <f>MIN(B2:B11)</f>
+        <v>666.24564536347998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14">
+        <f>MAX(B2:B11)</f>
+        <v>909.30577135828798</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15">
+        <f>AVERAGE(B2:B11)</f>
+        <v>753.39179493667314</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
done, still needs to be ready to send
</commit_message>
<xml_diff>
--- a/cbir/doc/kspecialclassifier.xlsx
+++ b/cbir/doc/kspecialclassifier.xlsx
@@ -4,22 +4,23 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="108" windowWidth="15120" windowHeight="8016" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="120" yWindow="108" windowWidth="15120" windowHeight="8016" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="K-Optimierung" sheetId="1" r:id="rId1"/>
     <sheet name="Min-Class-Size" sheetId="2" r:id="rId2"/>
     <sheet name="size" sheetId="3" r:id="rId3"/>
     <sheet name="K-Means-op" sheetId="4" r:id="rId4"/>
-    <sheet name="kspecial-op" sheetId="6" r:id="rId5"/>
-    <sheet name="kspecial-classify-op" sheetId="7" r:id="rId6"/>
+    <sheet name="kspecial-classify-op" sheetId="7" r:id="rId5"/>
+    <sheet name="kspecial-op" sheetId="6" r:id="rId6"/>
+    <sheet name="kspecial-op-result" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="38">
   <si>
     <t>K100</t>
   </si>
@@ -113,6 +114,27 @@
   <si>
     <t>Median</t>
   </si>
+  <si>
+    <t>Kspecial</t>
+  </si>
+  <si>
+    <t>With op</t>
+  </si>
+  <si>
+    <t>durchschn</t>
+  </si>
+  <si>
+    <t>with op</t>
+  </si>
+  <si>
+    <t>without</t>
+  </si>
+  <si>
+    <t>random only</t>
+  </si>
+  <si>
+    <t>1.7976931348623157E308</t>
+  </si>
 </sst>
 </file>
 
@@ -153,9 +175,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1824,382 +1847,1221 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:S44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView topLeftCell="C12" workbookViewId="0">
+      <selection activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="I1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
+        <v>23</v>
+      </c>
+      <c r="M1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2">
-        <v>88.235294117647001</v>
+        <v>98.039215686274503</v>
       </c>
       <c r="B2">
-        <v>754.17875115917104</v>
+        <v>729.04355200460805</v>
       </c>
       <c r="C2">
-        <v>8173</v>
+        <v>5662</v>
       </c>
       <c r="E2">
+        <v>74.509803921568604</v>
+      </c>
+      <c r="F2">
+        <v>809.33759080230595</v>
+      </c>
+      <c r="G2">
+        <v>6257</v>
+      </c>
+      <c r="I2">
         <v>80.392156862745097</v>
       </c>
-      <c r="F2">
-        <v>809.27234368397706</v>
-      </c>
-      <c r="G2">
-        <v>6137</v>
-      </c>
-      <c r="I2">
-        <v>88.235294117647001</v>
-      </c>
       <c r="J2">
-        <v>802.64742930456498</v>
+        <v>780.65094113417604</v>
       </c>
       <c r="K2">
-        <v>8116</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
+        <v>5946</v>
+      </c>
+      <c r="M2">
+        <v>92.156862745097996</v>
+      </c>
+      <c r="N2">
+        <v>810.07011520988499</v>
+      </c>
+      <c r="O2">
+        <v>6390</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3">
+        <v>92.156862745097996</v>
+      </c>
+      <c r="B3">
+        <v>822.37899622401198</v>
+      </c>
+      <c r="C3">
+        <v>6522</v>
+      </c>
+      <c r="E3">
+        <v>94.117647058823493</v>
+      </c>
+      <c r="F3">
+        <v>766.32998746276496</v>
+      </c>
+      <c r="G3">
+        <v>5155</v>
+      </c>
+      <c r="I3">
+        <v>80.392156862745097</v>
+      </c>
+      <c r="J3">
+        <v>807.41952804498101</v>
+      </c>
+      <c r="K3">
+        <v>5937</v>
+      </c>
+      <c r="M3">
         <v>86.274509803921504</v>
       </c>
-      <c r="B3">
-        <v>813.99997643713095</v>
-      </c>
-      <c r="C3">
-        <v>5089</v>
-      </c>
-      <c r="E3">
-        <v>92</v>
-      </c>
-      <c r="F3">
-        <v>764.88494690931498</v>
-      </c>
-      <c r="G3">
-        <v>6060</v>
-      </c>
-      <c r="I3">
-        <v>90.196078431372499</v>
-      </c>
-      <c r="J3">
-        <v>797.424723201284</v>
-      </c>
-      <c r="K3">
-        <v>6660</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+      <c r="N3">
+        <v>826.51509504967805</v>
+      </c>
+      <c r="O3">
+        <v>5972</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4">
-        <v>84.313725490196006</v>
+        <v>86</v>
       </c>
       <c r="B4">
-        <v>786.75135497350595</v>
+        <v>822.82340268697999</v>
       </c>
       <c r="C4">
-        <v>4563</v>
+        <v>5414</v>
       </c>
       <c r="E4">
-        <v>95.652173913043399</v>
+        <v>74.358974358974294</v>
       </c>
       <c r="F4">
-        <v>796.50245705101202</v>
+        <v>747.05909210359096</v>
       </c>
       <c r="G4">
-        <v>5519</v>
+        <v>6201</v>
       </c>
       <c r="I4">
-        <v>76</v>
+        <v>88.235294117647001</v>
       </c>
       <c r="J4">
-        <v>791.223120442908</v>
+        <v>881.77087279161901</v>
       </c>
       <c r="K4">
-        <v>6675</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
+        <v>7663</v>
+      </c>
+      <c r="M4">
+        <v>89.361702127659498</v>
+      </c>
+      <c r="N4">
+        <v>832.59502802417796</v>
+      </c>
+      <c r="O4">
+        <v>6796</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5">
-        <v>94.117647058823493</v>
+        <v>88.235294117647001</v>
       </c>
       <c r="B5">
-        <v>796.36046678316995</v>
+        <v>788.42654773099798</v>
       </c>
       <c r="C5">
-        <v>7999</v>
+        <v>6121</v>
       </c>
       <c r="E5">
-        <v>86</v>
+        <v>72.549019607843107</v>
       </c>
       <c r="F5">
-        <v>710.40592047357404</v>
+        <v>729.57791571502105</v>
       </c>
       <c r="G5">
-        <v>2174</v>
+        <v>2737</v>
       </c>
       <c r="I5">
         <v>86.274509803921504</v>
       </c>
       <c r="J5">
-        <v>755.11283076930897</v>
+        <v>761.59432397137402</v>
       </c>
       <c r="K5">
-        <v>7017</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
+        <v>8698</v>
+      </c>
+      <c r="M5">
+        <v>78.431372549019599</v>
+      </c>
+      <c r="N5">
+        <v>727.92763504012396</v>
+      </c>
+      <c r="O5">
+        <v>5811</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6">
-        <v>94.117647058823493</v>
+        <v>78.431372549019599</v>
       </c>
       <c r="B6">
-        <v>780.42362960139405</v>
+        <v>849.73860537320695</v>
       </c>
       <c r="C6">
-        <v>7907</v>
+        <v>5686</v>
       </c>
       <c r="E6">
-        <v>94</v>
+        <v>78.431372549019599</v>
       </c>
       <c r="F6">
-        <v>680.38336488072105</v>
+        <v>874.63961444061101</v>
       </c>
       <c r="G6">
-        <v>2781</v>
+        <v>6602</v>
       </c>
       <c r="I6">
-        <v>88.235294117647001</v>
+        <v>96.078431372549005</v>
       </c>
       <c r="J6">
-        <v>792.936091493964</v>
+        <v>790.59831809370405</v>
       </c>
       <c r="K6">
-        <v>7602</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
+        <v>5298</v>
+      </c>
+      <c r="M6">
+        <v>84.313725490196006</v>
+      </c>
+      <c r="N6">
+        <v>739.17893661983396</v>
+      </c>
+      <c r="O6">
+        <v>4340</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7">
+        <v>90.196078431372499</v>
+      </c>
+      <c r="B7">
+        <v>662.57072611009301</v>
+      </c>
+      <c r="C7">
+        <v>3276</v>
+      </c>
+      <c r="E7">
+        <v>92.156862745097996</v>
+      </c>
+      <c r="F7">
+        <v>711.51071463717005</v>
+      </c>
+      <c r="G7">
+        <v>2250</v>
+      </c>
+      <c r="I7">
         <v>80.392156862745097</v>
       </c>
-      <c r="B7">
-        <v>846.39928622112097</v>
-      </c>
-      <c r="C7">
-        <v>5703</v>
-      </c>
-      <c r="E7">
-        <v>90</v>
-      </c>
-      <c r="F7">
-        <v>655.30576788713904</v>
-      </c>
-      <c r="G7">
-        <v>2043</v>
-      </c>
-      <c r="I7">
-        <v>94.117647058823493</v>
-      </c>
       <c r="J7">
-        <v>878.40042309245905</v>
+        <v>805.02398235088197</v>
       </c>
       <c r="K7">
-        <v>9277</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
+        <v>10148</v>
+      </c>
+      <c r="M7">
+        <v>86.274509803921504</v>
+      </c>
+      <c r="N7">
+        <v>683.13176364621199</v>
+      </c>
+      <c r="O7">
+        <v>1751</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8">
+        <v>92.156862745097996</v>
+      </c>
+      <c r="B8">
+        <v>822.04187923323002</v>
+      </c>
+      <c r="C8">
+        <v>5848</v>
+      </c>
+      <c r="E8">
+        <v>88.235294117647001</v>
+      </c>
+      <c r="F8">
+        <v>713.89623498621404</v>
+      </c>
+      <c r="G8">
+        <v>2822</v>
+      </c>
+      <c r="I8">
+        <v>90.196078431372499</v>
+      </c>
+      <c r="J8">
+        <v>855.35191170923099</v>
+      </c>
+      <c r="K8">
+        <v>5483</v>
+      </c>
+      <c r="M8">
+        <v>82.352941176470495</v>
+      </c>
+      <c r="N8">
+        <v>725.070086752733</v>
+      </c>
+      <c r="O8">
+        <v>4761</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9">
+        <v>100</v>
+      </c>
+      <c r="B9">
+        <v>768.06390163748699</v>
+      </c>
+      <c r="C9">
+        <v>3100</v>
+      </c>
+      <c r="E9">
+        <v>90.196078431372499</v>
+      </c>
+      <c r="F9">
+        <v>821.90358612600699</v>
+      </c>
+      <c r="G9">
+        <v>6877</v>
+      </c>
+      <c r="I9">
+        <v>90.196078431372499</v>
+      </c>
+      <c r="J9">
+        <v>860.73319956724595</v>
+      </c>
+      <c r="K9">
+        <v>8004</v>
+      </c>
+      <c r="M9">
         <v>76.470588235294102</v>
       </c>
-      <c r="B8">
-        <v>848.94958115533495</v>
-      </c>
-      <c r="C8">
-        <v>4862</v>
-      </c>
-      <c r="E8">
-        <v>84.782608695652101</v>
-      </c>
-      <c r="F8">
-        <v>680.67753327961202</v>
-      </c>
-      <c r="G8">
-        <v>2108</v>
-      </c>
-      <c r="I8">
-        <v>76.470588235294102</v>
-      </c>
-      <c r="J8">
-        <v>775.63047066680895</v>
-      </c>
-      <c r="K8">
-        <v>6127</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
-      <c r="A9">
-        <v>90.196078431372499</v>
-      </c>
-      <c r="B9">
-        <v>859.99637531194503</v>
-      </c>
-      <c r="C9">
-        <v>4812</v>
-      </c>
-      <c r="E9">
-        <v>90.196078431372499</v>
-      </c>
-      <c r="F9">
-        <v>755.15960644572101</v>
-      </c>
-      <c r="G9">
-        <v>4475</v>
-      </c>
-      <c r="I9">
+      <c r="N9">
+        <v>722.58343200483102</v>
+      </c>
+      <c r="O9">
+        <v>3321</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10">
         <v>84.313725490196006</v>
       </c>
-      <c r="J9">
-        <v>746.07272242071895</v>
-      </c>
-      <c r="K9">
-        <v>5715</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
-      <c r="A10">
-        <v>88.235294117647001</v>
-      </c>
       <c r="B10">
-        <v>791.04380290533902</v>
+        <v>825.89823592861899</v>
       </c>
       <c r="C10">
-        <v>4506</v>
+        <v>5968</v>
       </c>
       <c r="E10">
-        <v>66.6666666666666</v>
+        <v>78.431372549019599</v>
       </c>
       <c r="F10">
-        <v>748.90724010269196</v>
+        <v>758.83258949342598</v>
       </c>
       <c r="G10">
-        <v>6561</v>
+        <v>3735</v>
       </c>
       <c r="I10">
-        <v>72.549019607843107</v>
+        <v>90.196078431372499</v>
       </c>
       <c r="J10">
-        <v>763.61098705775998</v>
+        <v>829.48182451681805</v>
       </c>
       <c r="K10">
-        <v>8680</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
+        <v>6321</v>
+      </c>
+      <c r="M10">
+        <v>88.235294117647001</v>
+      </c>
+      <c r="N10">
+        <v>803.63028708568004</v>
+      </c>
+      <c r="O10">
+        <v>6594</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
       <c r="A11">
-        <v>94.117647058823493</v>
+        <v>84.313725490196006</v>
       </c>
       <c r="B11">
-        <v>793.96834957876797</v>
+        <v>737.69041681339195</v>
       </c>
       <c r="C11">
-        <v>5233</v>
+        <v>4440</v>
       </c>
       <c r="E11">
-        <v>84.313725490196006</v>
+        <v>86.274509803921504</v>
       </c>
       <c r="F11">
-        <v>822.894730792985</v>
+        <v>801.81843155956994</v>
       </c>
       <c r="G11">
-        <v>5176</v>
+        <v>5681</v>
       </c>
       <c r="I11">
-        <v>92.156862745097996</v>
+        <v>82.352941176470495</v>
       </c>
       <c r="J11">
-        <v>804.91685267206003</v>
+        <v>761.26036555004998</v>
       </c>
       <c r="K11">
-        <v>6897</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
+        <v>6625</v>
+      </c>
+      <c r="M11">
+        <v>88.235294117647001</v>
+      </c>
+      <c r="N11">
+        <v>729.62182028704001</v>
+      </c>
+      <c r="O11">
+        <v>2404</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
       <c r="A13" t="s">
         <v>3</v>
       </c>
       <c r="B13">
-        <f>MIN(C2:C11)</f>
-        <v>4506</v>
+        <f>MIN(A2:A11)</f>
+        <v>78.431372549019599</v>
       </c>
       <c r="E13" t="s">
         <v>3</v>
       </c>
       <c r="F13">
-        <f>MIN(G2:G11)</f>
-        <v>2043</v>
+        <f>MIN(E2:E11)</f>
+        <v>72.549019607843107</v>
       </c>
       <c r="I13" t="s">
         <v>3</v>
       </c>
       <c r="J13">
-        <f>MIN(K2:K11)</f>
-        <v>5715</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11">
+        <f>MIN(I2:I11)</f>
+        <v>80.392156862745097</v>
+      </c>
+      <c r="M13" t="s">
+        <v>3</v>
+      </c>
+      <c r="N13">
+        <f>MIN(M2:M11)</f>
+        <v>76.470588235294102</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
       <c r="A14" t="s">
         <v>4</v>
       </c>
       <c r="B14">
-        <f>MAX(C2:C11)</f>
-        <v>8173</v>
+        <f>MAX(A2:A11)</f>
+        <v>100</v>
       </c>
       <c r="E14" t="s">
         <v>4</v>
       </c>
       <c r="F14">
-        <f>MAX(G2:G11)</f>
-        <v>6561</v>
+        <f>MAX(E2:E11)</f>
+        <v>94.117647058823493</v>
       </c>
       <c r="I14" t="s">
         <v>4</v>
       </c>
       <c r="J14">
-        <f>MAX(K2:K11)</f>
-        <v>9277</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11">
+        <f>MAX(I2:I11)</f>
+        <v>96.078431372549005</v>
+      </c>
+      <c r="M14" t="s">
+        <v>4</v>
+      </c>
+      <c r="N14">
+        <f>MAX(M2:M11)</f>
+        <v>92.156862745097996</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
       <c r="A15" t="s">
         <v>5</v>
       </c>
       <c r="B15">
-        <f>AVERAGE(C2:C11)</f>
-        <v>5884.7</v>
+        <f>AVERAGE(A2:A11)</f>
+        <v>89.384313725490159</v>
       </c>
       <c r="E15" t="s">
         <v>5</v>
       </c>
       <c r="F15">
-        <f>AVERAGE(G2:G11)</f>
-        <v>4303.3999999999996</v>
+        <f>AVERAGE(E2:E11)</f>
+        <v>82.92609351432877</v>
       </c>
       <c r="I15" t="s">
         <v>5</v>
       </c>
       <c r="J15">
-        <f>AVERAGE(K2:K11)</f>
-        <v>7276.6</v>
+        <f>AVERAGE(I2:I11)</f>
+        <v>86.470588235294073</v>
+      </c>
+      <c r="M15" t="s">
+        <v>5</v>
+      </c>
+      <c r="N15">
+        <f>AVERAGE(M2:M11)</f>
+        <v>85.210680016687462</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="B16">
+        <f>MEDIAN(A2:A11)</f>
+        <v>89.21568627450975</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19">
+      <c r="A18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19">
+      <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="E19" t="s">
+        <v>27</v>
+      </c>
+      <c r="I19" t="s">
+        <v>28</v>
+      </c>
+      <c r="M19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19">
+      <c r="A20">
+        <v>94.117647058823493</v>
+      </c>
+      <c r="B20">
+        <v>770.17312879989595</v>
+      </c>
+      <c r="C20">
+        <v>4970</v>
+      </c>
+      <c r="E20">
+        <v>96.078431372549005</v>
+      </c>
+      <c r="F20">
+        <v>749.39526821672803</v>
+      </c>
+      <c r="G20">
+        <v>4638</v>
+      </c>
+      <c r="I20">
+        <v>82.352941176470495</v>
+      </c>
+      <c r="J20">
+        <v>781.66938288194103</v>
+      </c>
+      <c r="K20">
+        <v>4369</v>
+      </c>
+      <c r="M20">
+        <v>80.392156862745097</v>
+      </c>
+      <c r="N20">
+        <v>791.07893334927599</v>
+      </c>
+      <c r="O20">
+        <v>4804</v>
+      </c>
+      <c r="Q20">
+        <v>90.196078431372499</v>
+      </c>
+      <c r="R20">
+        <v>756.58171239316403</v>
+      </c>
+      <c r="S20">
+        <v>4285</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19">
+      <c r="A21">
+        <v>98.039215686274503</v>
+      </c>
+      <c r="B21">
+        <v>795.39246679357495</v>
+      </c>
+      <c r="C21">
+        <v>7077</v>
+      </c>
+      <c r="E21">
+        <v>80.392156862745097</v>
+      </c>
+      <c r="F21">
+        <v>772.19734793571104</v>
+      </c>
+      <c r="G21">
+        <v>6569</v>
+      </c>
+      <c r="I21">
+        <v>72.549019607843107</v>
+      </c>
+      <c r="J21">
+        <v>857.40650350734802</v>
+      </c>
+      <c r="K21">
+        <v>4710</v>
+      </c>
+      <c r="M21">
+        <v>94.117647058823493</v>
+      </c>
+      <c r="N21">
+        <v>762.73930525252899</v>
+      </c>
+      <c r="O21">
+        <v>5741</v>
+      </c>
+      <c r="Q21">
+        <v>98.039215686274503</v>
+      </c>
+      <c r="R21">
+        <v>820.11334015214004</v>
+      </c>
+      <c r="S21">
+        <v>5372</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19">
+      <c r="A22">
+        <v>92.156862745097996</v>
+      </c>
+      <c r="B22">
+        <v>795.37105044782504</v>
+      </c>
+      <c r="C22">
+        <v>7382</v>
+      </c>
+      <c r="E22">
+        <v>95</v>
+      </c>
+      <c r="F22">
+        <v>729.54464574009501</v>
+      </c>
+      <c r="G22">
+        <v>5075</v>
+      </c>
+      <c r="I22">
+        <v>82</v>
+      </c>
+      <c r="J22">
+        <v>784.68793293114197</v>
+      </c>
+      <c r="K22">
+        <v>6017</v>
+      </c>
+      <c r="M22">
+        <v>96.078431372549005</v>
+      </c>
+      <c r="N22">
+        <v>796.36040756301804</v>
+      </c>
+      <c r="O22">
+        <v>6301</v>
+      </c>
+      <c r="Q22">
+        <v>76</v>
+      </c>
+      <c r="R22">
+        <v>786.34411094422603</v>
+      </c>
+      <c r="S22">
+        <v>4829</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19">
+      <c r="A23">
+        <v>86.274509803921504</v>
+      </c>
+      <c r="B23">
+        <v>740.67952674033904</v>
+      </c>
+      <c r="C23">
+        <v>5088</v>
+      </c>
+      <c r="E23">
+        <v>80.392156862745097</v>
+      </c>
+      <c r="F23">
+        <v>721.51809992752601</v>
+      </c>
+      <c r="G23">
+        <v>1833</v>
+      </c>
+      <c r="I23">
+        <v>90.196078431372499</v>
+      </c>
+      <c r="J23">
+        <v>784.47282623287299</v>
+      </c>
+      <c r="K23">
+        <v>5726</v>
+      </c>
+      <c r="M23">
+        <v>82.352941176470495</v>
+      </c>
+      <c r="N23">
+        <v>774.37243739302005</v>
+      </c>
+      <c r="O23">
+        <v>5822</v>
+      </c>
+      <c r="Q23">
+        <v>94.117647058823493</v>
+      </c>
+      <c r="R23">
+        <v>719.61111819309099</v>
+      </c>
+      <c r="S23">
+        <v>8832</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19">
+      <c r="A24">
+        <v>90.196078431372499</v>
+      </c>
+      <c r="B24">
+        <v>812.61298302316197</v>
+      </c>
+      <c r="C24">
+        <v>6335</v>
+      </c>
+      <c r="E24">
+        <v>86.274509803921504</v>
+      </c>
+      <c r="F24">
+        <v>728.79793710737101</v>
+      </c>
+      <c r="G24">
+        <v>2576</v>
+      </c>
+      <c r="I24">
+        <v>86.274509803921504</v>
+      </c>
+      <c r="J24">
+        <v>717.69898206713901</v>
+      </c>
+      <c r="K24">
+        <v>2415</v>
+      </c>
+      <c r="M24">
+        <v>84.313725490196006</v>
+      </c>
+      <c r="N24">
+        <v>853.60195246338503</v>
+      </c>
+      <c r="O24">
+        <v>7507</v>
+      </c>
+      <c r="Q24">
+        <v>88.235294117647001</v>
+      </c>
+      <c r="R24">
+        <v>768.62483023664402</v>
+      </c>
+      <c r="S24">
+        <v>5891</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19">
+      <c r="A25">
+        <v>86.274509803921504</v>
+      </c>
+      <c r="B25">
+        <v>748.15799519418601</v>
+      </c>
+      <c r="C25">
+        <v>6599</v>
+      </c>
+      <c r="E25">
+        <v>90.196078431372499</v>
+      </c>
+      <c r="F25">
+        <v>653.84359191098099</v>
+      </c>
+      <c r="G25">
+        <v>963</v>
+      </c>
+      <c r="I25">
+        <v>90.196078431372499</v>
+      </c>
+      <c r="J25">
+        <v>753.71662282548596</v>
+      </c>
+      <c r="K25">
+        <v>5243</v>
+      </c>
+      <c r="M25">
+        <v>90.196078431372499</v>
+      </c>
+      <c r="N25">
+        <v>770.64711124827204</v>
+      </c>
+      <c r="O25">
+        <v>5507</v>
+      </c>
+      <c r="Q25">
+        <v>90.196078431372499</v>
+      </c>
+      <c r="R25">
+        <v>844.44138264222704</v>
+      </c>
+      <c r="S25">
+        <v>5733</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19">
+      <c r="A26">
+        <v>88.235294117647001</v>
+      </c>
+      <c r="B26">
+        <v>792.39225961073396</v>
+      </c>
+      <c r="C26">
+        <v>4911</v>
+      </c>
+      <c r="E26">
+        <v>92.156862745097996</v>
+      </c>
+      <c r="F26">
+        <v>714.76255657235504</v>
+      </c>
+      <c r="G26">
+        <v>3214</v>
+      </c>
+      <c r="I26">
+        <v>84.313725490196006</v>
+      </c>
+      <c r="J26">
+        <v>832.43274089894601</v>
+      </c>
+      <c r="K26">
+        <v>6814</v>
+      </c>
+      <c r="M26">
+        <v>96.078431372549005</v>
+      </c>
+      <c r="N26">
+        <v>770.470562127074</v>
+      </c>
+      <c r="O26">
+        <v>5612</v>
+      </c>
+      <c r="Q26">
+        <v>76.470588235294102</v>
+      </c>
+      <c r="R26">
+        <v>931.16422197632903</v>
+      </c>
+      <c r="S26">
+        <v>6843</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19">
+      <c r="A27">
+        <v>88.235294117647001</v>
+      </c>
+      <c r="B27">
+        <v>819.94413613193103</v>
+      </c>
+      <c r="C27">
+        <v>5068</v>
+      </c>
+      <c r="E27">
+        <v>86.274509803921504</v>
+      </c>
+      <c r="F27">
+        <v>781.74246210550598</v>
+      </c>
+      <c r="G27">
+        <v>5765</v>
+      </c>
+      <c r="I27">
+        <v>86.274509803921504</v>
+      </c>
+      <c r="J27">
+        <v>831.833241900453</v>
+      </c>
+      <c r="K27">
+        <v>5405</v>
+      </c>
+      <c r="M27">
+        <v>88.235294117647001</v>
+      </c>
+      <c r="N27">
+        <v>733.24608544498199</v>
+      </c>
+      <c r="O27">
+        <v>5924</v>
+      </c>
+      <c r="Q27">
+        <v>88.235294117647001</v>
+      </c>
+      <c r="R27">
+        <v>874.41508906403101</v>
+      </c>
+      <c r="S27">
+        <v>5387</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19">
+      <c r="A28">
+        <v>82.352941176470495</v>
+      </c>
+      <c r="B28">
+        <v>783.27148625442101</v>
+      </c>
+      <c r="C28">
+        <v>6628</v>
+      </c>
+      <c r="E28">
+        <v>94.117647058823493</v>
+      </c>
+      <c r="F28">
+        <v>827.25439537822297</v>
+      </c>
+      <c r="G28">
+        <v>5775</v>
+      </c>
+      <c r="I28">
+        <v>90.196078431372499</v>
+      </c>
+      <c r="J28">
+        <v>818.84339887792805</v>
+      </c>
+      <c r="K28">
+        <v>5773</v>
+      </c>
+      <c r="M28">
+        <v>88.235294117647001</v>
+      </c>
+      <c r="N28">
+        <v>739.37913831708397</v>
+      </c>
+      <c r="O28">
+        <v>3545</v>
+      </c>
+      <c r="Q28">
+        <v>90.196078431372499</v>
+      </c>
+      <c r="R28">
+        <v>847.00532203181899</v>
+      </c>
+      <c r="S28">
+        <v>6260</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19">
+      <c r="A29">
+        <v>82.352941176470495</v>
+      </c>
+      <c r="B29">
+        <v>843.02185636310401</v>
+      </c>
+      <c r="C29">
+        <v>4813</v>
+      </c>
+      <c r="E29">
+        <v>84.313725490196006</v>
+      </c>
+      <c r="F29">
+        <v>809.83399915048301</v>
+      </c>
+      <c r="G29">
+        <v>4866</v>
+      </c>
+      <c r="I29">
+        <v>76.470588235294102</v>
+      </c>
+      <c r="J29">
+        <v>776.99092006283797</v>
+      </c>
+      <c r="K29">
+        <v>4535</v>
+      </c>
+      <c r="M29">
+        <v>90.196078431372499</v>
+      </c>
+      <c r="N29">
+        <v>760.90801855924406</v>
+      </c>
+      <c r="O29">
+        <v>6263</v>
+      </c>
+      <c r="Q29">
+        <v>94.117647058823493</v>
+      </c>
+      <c r="R29">
+        <v>830.35268415934104</v>
+      </c>
+      <c r="S29">
+        <v>5005</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19">
+      <c r="Q30">
+        <v>90.196078431372499</v>
+      </c>
+      <c r="R30">
+        <v>787.70666282135801</v>
+      </c>
+      <c r="S30">
+        <v>13257</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19">
+      <c r="A31" t="s">
+        <v>3</v>
+      </c>
+      <c r="B31">
+        <f>MIN(A20:A29)</f>
+        <v>82.352941176470495</v>
+      </c>
+      <c r="E31" t="s">
+        <v>3</v>
+      </c>
+      <c r="F31">
+        <f>MIN(E20:E29)</f>
+        <v>80.392156862745097</v>
+      </c>
+      <c r="I31" t="s">
+        <v>3</v>
+      </c>
+      <c r="J31">
+        <f>MIN(I20:I29)</f>
+        <v>72.549019607843107</v>
+      </c>
+      <c r="M31" t="s">
+        <v>3</v>
+      </c>
+      <c r="N31">
+        <f>MIN(M20:M29)</f>
+        <v>80.392156862745097</v>
+      </c>
+      <c r="Q31">
+        <v>74.509803921568604</v>
+      </c>
+      <c r="R31">
+        <v>892.39361398721906</v>
+      </c>
+      <c r="S31">
+        <v>5273</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19">
+      <c r="A32" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32">
+        <f>MAX(A20:A29)</f>
+        <v>98.039215686274503</v>
+      </c>
+      <c r="E32" t="s">
+        <v>4</v>
+      </c>
+      <c r="F32">
+        <f>MAX(E20:E29)</f>
+        <v>96.078431372549005</v>
+      </c>
+      <c r="I32" t="s">
+        <v>4</v>
+      </c>
+      <c r="J32">
+        <f>MAX(I20:I29)</f>
+        <v>90.196078431372499</v>
+      </c>
+      <c r="M32" t="s">
+        <v>4</v>
+      </c>
+      <c r="N32">
+        <f>MAX(M20:M29)</f>
+        <v>96.078431372549005</v>
+      </c>
+      <c r="Q32">
+        <v>90.196078431372499</v>
+      </c>
+      <c r="R32">
+        <v>808.38680182663097</v>
+      </c>
+      <c r="S32">
+        <v>11731</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19">
+      <c r="A33" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33">
+        <f>AVERAGE(A20:A29)</f>
+        <v>88.823529411764639</v>
+      </c>
+      <c r="E33" t="s">
+        <v>5</v>
+      </c>
+      <c r="F33">
+        <f>AVERAGE(E20:E29)</f>
+        <v>88.519607843137223</v>
+      </c>
+      <c r="I33" t="s">
+        <v>5</v>
+      </c>
+      <c r="J33">
+        <f>AVERAGE(I20:I29)</f>
+        <v>84.082352941176424</v>
+      </c>
+      <c r="M33" t="s">
+        <v>5</v>
+      </c>
+      <c r="N33">
+        <f>AVERAGE(M20:M29)</f>
+        <v>89.019607843137209</v>
+      </c>
+      <c r="Q33">
+        <v>94.117647058823493</v>
+      </c>
+      <c r="R33">
+        <v>729.85457422329102</v>
+      </c>
+      <c r="S33">
+        <v>4206</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19">
+      <c r="Q34">
+        <v>84.313725490196006</v>
+      </c>
+      <c r="R34">
+        <v>843.03460671236803</v>
+      </c>
+      <c r="S34">
+        <v>5834</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19">
+      <c r="Q35">
+        <v>88.235294117647001</v>
+      </c>
+      <c r="R35">
+        <v>826.287500786279</v>
+      </c>
+      <c r="S35">
+        <v>6844</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19">
+      <c r="Q36">
+        <v>94.117647058823493</v>
+      </c>
+      <c r="R36">
+        <v>790.47650635060495</v>
+      </c>
+      <c r="S36">
+        <v>5266</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19">
+      <c r="Q37">
+        <v>86.274509803921504</v>
+      </c>
+      <c r="R37">
+        <v>753.14397739178503</v>
+      </c>
+      <c r="S37">
+        <v>3814</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19">
+      <c r="Q38">
+        <v>96.078431372549005</v>
+      </c>
+      <c r="R38">
+        <v>788.72538952217803</v>
+      </c>
+      <c r="S38">
+        <v>5433</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19">
+      <c r="Q39">
+        <v>90.196078431372499</v>
+      </c>
+      <c r="R39">
+        <v>809.09418052815499</v>
+      </c>
+      <c r="S39">
+        <v>5957</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19">
+      <c r="Q41" t="s">
+        <v>3</v>
+      </c>
+      <c r="R41">
+        <f>MIN(Q20:Q39)</f>
+        <v>74.509803921568604</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19">
+      <c r="Q42" t="s">
+        <v>4</v>
+      </c>
+      <c r="R42">
+        <f>MAX(Q20:Q39)</f>
+        <v>98.039215686274503</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19">
+      <c r="Q43" t="s">
+        <v>33</v>
+      </c>
+      <c r="R43">
+        <f>AVERAGE(Q20:Q39)</f>
+        <v>88.701960784313684</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19">
+      <c r="Q44" t="s">
+        <v>29</v>
+      </c>
+      <c r="R44">
+        <f>MEDIAN(Q20:Q39)</f>
+        <v>90.196078431372499</v>
       </c>
     </row>
   </sheetData>
@@ -2209,406 +3071,406 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S44"/>
+  <dimension ref="A1:O18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C16" workbookViewId="0">
-      <selection activeCell="Q43" sqref="Q43"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M2" sqref="M2:O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:15">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="M1" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:15">
       <c r="A2">
-        <v>98.039215686274503</v>
+        <v>88.235294117647001</v>
       </c>
       <c r="B2">
-        <v>729.04355200460805</v>
+        <v>754.17875115917104</v>
       </c>
       <c r="C2">
-        <v>5662</v>
+        <v>8173</v>
       </c>
       <c r="E2">
-        <v>74.509803921568604</v>
+        <v>80.392156862745097</v>
       </c>
       <c r="F2">
-        <v>809.33759080230595</v>
+        <v>809.27234368397706</v>
       </c>
       <c r="G2">
-        <v>6257</v>
+        <v>6137</v>
       </c>
       <c r="I2">
-        <v>80.392156862745097</v>
+        <v>88.235294117647001</v>
       </c>
       <c r="J2">
-        <v>780.65094113417604</v>
+        <v>802.64742930456498</v>
       </c>
       <c r="K2">
-        <v>5946</v>
+        <v>8116</v>
       </c>
       <c r="M2">
-        <v>92.156862745097996</v>
+        <v>88.235294117647001</v>
       </c>
       <c r="N2">
-        <v>810.07011520988499</v>
+        <v>759.44715604235398</v>
       </c>
       <c r="O2">
-        <v>6390</v>
+        <v>4285</v>
       </c>
     </row>
     <row r="3" spans="1:15">
       <c r="A3">
-        <v>92.156862745097996</v>
+        <v>86.274509803921504</v>
       </c>
       <c r="B3">
-        <v>822.37899622401198</v>
+        <v>813.99997643713095</v>
       </c>
       <c r="C3">
-        <v>6522</v>
+        <v>5089</v>
       </c>
       <c r="E3">
-        <v>94.117647058823493</v>
+        <v>92</v>
       </c>
       <c r="F3">
-        <v>766.32998746276496</v>
+        <v>764.88494690931498</v>
       </c>
       <c r="G3">
-        <v>5155</v>
+        <v>6060</v>
       </c>
       <c r="I3">
-        <v>80.392156862745097</v>
+        <v>90.196078431372499</v>
       </c>
       <c r="J3">
-        <v>807.41952804498101</v>
+        <v>797.424723201284</v>
       </c>
       <c r="K3">
-        <v>5937</v>
+        <v>6660</v>
       </c>
       <c r="M3">
-        <v>86.274509803921504</v>
+        <v>88.235294117647001</v>
       </c>
       <c r="N3">
-        <v>826.51509504967805</v>
+        <v>827.75398833418899</v>
       </c>
       <c r="O3">
-        <v>5972</v>
+        <v>6418</v>
       </c>
     </row>
     <row r="4" spans="1:15">
       <c r="A4">
-        <v>86</v>
+        <v>84.313725490196006</v>
       </c>
       <c r="B4">
-        <v>822.82340268697999</v>
+        <v>786.75135497350595</v>
       </c>
       <c r="C4">
-        <v>5414</v>
+        <v>4563</v>
       </c>
       <c r="E4">
-        <v>74.358974358974294</v>
+        <v>95.652173913043399</v>
       </c>
       <c r="F4">
-        <v>747.05909210359096</v>
+        <v>796.50245705101202</v>
       </c>
       <c r="G4">
-        <v>6201</v>
+        <v>5519</v>
       </c>
       <c r="I4">
-        <v>88.235294117647001</v>
+        <v>76</v>
       </c>
       <c r="J4">
-        <v>881.77087279161901</v>
+        <v>791.223120442908</v>
       </c>
       <c r="K4">
-        <v>7663</v>
+        <v>6675</v>
       </c>
       <c r="M4">
-        <v>89.361702127659498</v>
+        <v>88.235294117647001</v>
       </c>
       <c r="N4">
-        <v>832.59502802417796</v>
+        <v>782.45089824684396</v>
       </c>
       <c r="O4">
-        <v>6796</v>
+        <v>5575</v>
       </c>
     </row>
     <row r="5" spans="1:15">
       <c r="A5">
-        <v>88.235294117647001</v>
+        <v>94.117647058823493</v>
       </c>
       <c r="B5">
-        <v>788.42654773099798</v>
+        <v>796.36046678316995</v>
       </c>
       <c r="C5">
-        <v>6121</v>
+        <v>7999</v>
       </c>
       <c r="E5">
-        <v>72.549019607843107</v>
+        <v>86</v>
       </c>
       <c r="F5">
-        <v>729.57791571502105</v>
+        <v>710.40592047357404</v>
       </c>
       <c r="G5">
-        <v>2737</v>
+        <v>2174</v>
       </c>
       <c r="I5">
         <v>86.274509803921504</v>
       </c>
       <c r="J5">
-        <v>761.59432397137402</v>
+        <v>755.11283076930897</v>
       </c>
       <c r="K5">
-        <v>8698</v>
+        <v>7017</v>
       </c>
       <c r="M5">
-        <v>78.431372549019599</v>
+        <v>86.274509803921504</v>
       </c>
       <c r="N5">
-        <v>727.92763504012396</v>
+        <v>764.576396249666</v>
       </c>
       <c r="O5">
-        <v>5811</v>
+        <v>4186</v>
       </c>
     </row>
     <row r="6" spans="1:15">
       <c r="A6">
-        <v>78.431372549019599</v>
+        <v>94.117647058823493</v>
       </c>
       <c r="B6">
-        <v>849.73860537320695</v>
+        <v>780.42362960139405</v>
       </c>
       <c r="C6">
-        <v>5686</v>
+        <v>7907</v>
       </c>
       <c r="E6">
-        <v>78.431372549019599</v>
+        <v>94</v>
       </c>
       <c r="F6">
-        <v>874.63961444061101</v>
+        <v>680.38336488072105</v>
       </c>
       <c r="G6">
-        <v>6602</v>
+        <v>2781</v>
       </c>
       <c r="I6">
-        <v>96.078431372549005</v>
+        <v>88.235294117647001</v>
       </c>
       <c r="J6">
-        <v>790.59831809370405</v>
+        <v>792.936091493964</v>
       </c>
       <c r="K6">
-        <v>5298</v>
+        <v>7602</v>
       </c>
       <c r="M6">
-        <v>84.313725490196006</v>
+        <v>88.235294117647001</v>
       </c>
       <c r="N6">
-        <v>739.17893661983396</v>
+        <v>713.37898004405395</v>
       </c>
       <c r="O6">
-        <v>4340</v>
+        <v>2115</v>
       </c>
     </row>
     <row r="7" spans="1:15">
       <c r="A7">
-        <v>90.196078431372499</v>
+        <v>80.392156862745097</v>
       </c>
       <c r="B7">
-        <v>662.57072611009301</v>
+        <v>846.39928622112097</v>
       </c>
       <c r="C7">
-        <v>3276</v>
+        <v>5703</v>
       </c>
       <c r="E7">
-        <v>92.156862745097996</v>
+        <v>90</v>
       </c>
       <c r="F7">
-        <v>711.51071463717005</v>
+        <v>655.30576788713904</v>
       </c>
       <c r="G7">
-        <v>2250</v>
+        <v>2043</v>
       </c>
       <c r="I7">
-        <v>80.392156862745097</v>
+        <v>94.117647058823493</v>
       </c>
       <c r="J7">
-        <v>805.02398235088197</v>
+        <v>878.40042309245905</v>
       </c>
       <c r="K7">
-        <v>10148</v>
+        <v>9277</v>
       </c>
       <c r="M7">
-        <v>86.274509803921504</v>
+        <v>88.235294117647001</v>
       </c>
       <c r="N7">
-        <v>683.13176364621199</v>
+        <v>721.38397425202402</v>
       </c>
       <c r="O7">
-        <v>1751</v>
+        <v>2183</v>
       </c>
     </row>
     <row r="8" spans="1:15">
       <c r="A8">
-        <v>92.156862745097996</v>
+        <v>76.470588235294102</v>
       </c>
       <c r="B8">
-        <v>822.04187923323002</v>
+        <v>848.94958115533495</v>
       </c>
       <c r="C8">
-        <v>5848</v>
+        <v>4862</v>
       </c>
       <c r="E8">
-        <v>88.235294117647001</v>
+        <v>84.782608695652101</v>
       </c>
       <c r="F8">
-        <v>713.89623498621404</v>
+        <v>680.67753327961202</v>
       </c>
       <c r="G8">
-        <v>2822</v>
+        <v>2108</v>
       </c>
       <c r="I8">
-        <v>90.196078431372499</v>
+        <v>76.470588235294102</v>
       </c>
       <c r="J8">
-        <v>855.35191170923099</v>
+        <v>775.63047066680895</v>
       </c>
       <c r="K8">
-        <v>5483</v>
+        <v>6127</v>
       </c>
       <c r="M8">
-        <v>82.352941176470495</v>
+        <v>74.509803921568604</v>
       </c>
       <c r="N8">
-        <v>725.070086752733</v>
+        <v>823.94856350048406</v>
       </c>
       <c r="O8">
-        <v>4761</v>
+        <v>6471</v>
       </c>
     </row>
     <row r="9" spans="1:15">
       <c r="A9">
-        <v>100</v>
+        <v>90.196078431372499</v>
       </c>
       <c r="B9">
-        <v>768.06390163748699</v>
+        <v>859.99637531194503</v>
       </c>
       <c r="C9">
-        <v>3100</v>
+        <v>4812</v>
       </c>
       <c r="E9">
         <v>90.196078431372499</v>
       </c>
       <c r="F9">
-        <v>821.90358612600699</v>
+        <v>755.15960644572101</v>
       </c>
       <c r="G9">
-        <v>6877</v>
+        <v>4475</v>
       </c>
       <c r="I9">
-        <v>90.196078431372499</v>
+        <v>84.313725490196006</v>
       </c>
       <c r="J9">
-        <v>860.73319956724595</v>
+        <v>746.07272242071895</v>
       </c>
       <c r="K9">
-        <v>8004</v>
+        <v>5715</v>
       </c>
       <c r="M9">
-        <v>76.470588235294102</v>
+        <v>94.117647058823493</v>
       </c>
       <c r="N9">
-        <v>722.58343200483102</v>
+        <v>740.35580196833098</v>
       </c>
       <c r="O9">
-        <v>3321</v>
+        <v>5740</v>
       </c>
     </row>
     <row r="10" spans="1:15">
       <c r="A10">
-        <v>84.313725490196006</v>
+        <v>88.235294117647001</v>
       </c>
       <c r="B10">
-        <v>825.89823592861899</v>
+        <v>791.04380290533902</v>
       </c>
       <c r="C10">
-        <v>5968</v>
+        <v>4506</v>
       </c>
       <c r="E10">
-        <v>78.431372549019599</v>
+        <v>66.6666666666666</v>
       </c>
       <c r="F10">
-        <v>758.83258949342598</v>
+        <v>748.90724010269196</v>
       </c>
       <c r="G10">
-        <v>3735</v>
+        <v>6561</v>
       </c>
       <c r="I10">
-        <v>90.196078431372499</v>
+        <v>72.549019607843107</v>
       </c>
       <c r="J10">
-        <v>829.48182451681805</v>
+        <v>763.61098705775998</v>
       </c>
       <c r="K10">
-        <v>6321</v>
+        <v>8680</v>
       </c>
       <c r="M10">
-        <v>88.235294117647001</v>
+        <v>100</v>
       </c>
       <c r="N10">
-        <v>803.63028708568004</v>
+        <v>809.977626068007</v>
       </c>
       <c r="O10">
-        <v>6594</v>
+        <v>6115</v>
       </c>
     </row>
     <row r="11" spans="1:15">
       <c r="A11">
+        <v>94.117647058823493</v>
+      </c>
+      <c r="B11">
+        <v>793.96834957876797</v>
+      </c>
+      <c r="C11">
+        <v>5233</v>
+      </c>
+      <c r="E11">
         <v>84.313725490196006</v>
       </c>
-      <c r="B11">
-        <v>737.69041681339195</v>
-      </c>
-      <c r="C11">
-        <v>4440</v>
-      </c>
-      <c r="E11">
-        <v>86.274509803921504</v>
-      </c>
       <c r="F11">
-        <v>801.81843155956994</v>
+        <v>822.894730792985</v>
       </c>
       <c r="G11">
-        <v>5681</v>
+        <v>5176</v>
       </c>
       <c r="I11">
-        <v>82.352941176470495</v>
+        <v>92.156862745097996</v>
       </c>
       <c r="J11">
-        <v>761.26036555004998</v>
+        <v>804.91685267206003</v>
       </c>
       <c r="K11">
-        <v>6625</v>
+        <v>6897</v>
       </c>
       <c r="M11">
-        <v>88.235294117647001</v>
+        <v>78.431372549019599</v>
       </c>
       <c r="N11">
-        <v>729.62182028704001</v>
+        <v>765.784224228364</v>
       </c>
       <c r="O11">
-        <v>2404</v>
+        <v>3257</v>
       </c>
     </row>
     <row r="13" spans="1:15">
@@ -2616,29 +3478,29 @@
         <v>3</v>
       </c>
       <c r="B13">
-        <f>MIN(A2:A11)</f>
-        <v>78.431372549019599</v>
+        <f>MIN(C2:C11)</f>
+        <v>4506</v>
       </c>
       <c r="E13" t="s">
         <v>3</v>
       </c>
       <c r="F13">
-        <f>MIN(E2:E11)</f>
-        <v>72.549019607843107</v>
+        <f>MIN(G2:G11)</f>
+        <v>2043</v>
       </c>
       <c r="I13" t="s">
         <v>3</v>
       </c>
       <c r="J13">
-        <f>MIN(I2:I11)</f>
-        <v>80.392156862745097</v>
+        <f>MIN(K2:K11)</f>
+        <v>5715</v>
       </c>
       <c r="M13" t="s">
         <v>3</v>
       </c>
       <c r="N13">
-        <f>MIN(M2:M11)</f>
-        <v>76.470588235294102</v>
+        <f>MIN(O2:O11)</f>
+        <v>2115</v>
       </c>
     </row>
     <row r="14" spans="1:15">
@@ -2646,29 +3508,29 @@
         <v>4</v>
       </c>
       <c r="B14">
-        <f>MAX(A2:A11)</f>
-        <v>100</v>
+        <f>MAX(C2:C11)</f>
+        <v>8173</v>
       </c>
       <c r="E14" t="s">
         <v>4</v>
       </c>
       <c r="F14">
-        <f>MAX(E2:E11)</f>
-        <v>94.117647058823493</v>
+        <f>MAX(G2:G11)</f>
+        <v>6561</v>
       </c>
       <c r="I14" t="s">
         <v>4</v>
       </c>
       <c r="J14">
-        <f>MAX(I2:I11)</f>
-        <v>96.078431372549005</v>
+        <f>MAX(K2:K11)</f>
+        <v>9277</v>
       </c>
       <c r="M14" t="s">
         <v>4</v>
       </c>
       <c r="N14">
-        <f>MAX(M2:M11)</f>
-        <v>92.156862745097996</v>
+        <f>MAX(O2:O11)</f>
+        <v>6471</v>
       </c>
     </row>
     <row r="15" spans="1:15">
@@ -2676,745 +3538,757 @@
         <v>5</v>
       </c>
       <c r="B15">
-        <f>AVERAGE(A2:A11)</f>
-        <v>89.384313725490159</v>
+        <f>AVERAGE(C2:C11)</f>
+        <v>5884.7</v>
       </c>
       <c r="E15" t="s">
         <v>5</v>
       </c>
       <c r="F15">
-        <f>AVERAGE(E2:E11)</f>
-        <v>82.92609351432877</v>
+        <f>AVERAGE(G2:G11)</f>
+        <v>4303.3999999999996</v>
       </c>
       <c r="I15" t="s">
         <v>5</v>
       </c>
       <c r="J15">
-        <f>AVERAGE(I2:I11)</f>
-        <v>86.470588235294073</v>
+        <f>AVERAGE(K2:K11)</f>
+        <v>7276.6</v>
       </c>
       <c r="M15" t="s">
         <v>5</v>
       </c>
       <c r="N15">
+        <f>AVERAGE(O2:O11)</f>
+        <v>4634.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="M16" t="s">
+        <v>3</v>
+      </c>
+      <c r="N16">
+        <f>MIN(M2:M11)</f>
+        <v>74.509803921568604</v>
+      </c>
+    </row>
+    <row r="17" spans="13:14">
+      <c r="M17" t="s">
+        <v>4</v>
+      </c>
+      <c r="N17">
+        <f>MAX(M2:M11)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="13:14">
+      <c r="M18" t="s">
+        <v>5</v>
+      </c>
+      <c r="N18">
         <f>AVERAGE(M2:M11)</f>
-        <v>85.210680016687462</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15">
+        <v>87.450980392156822</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:K26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L27" sqref="L27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2">
+        <v>88.235294117647001</v>
+      </c>
+      <c r="B2">
+        <v>759.44715604235398</v>
+      </c>
+      <c r="C2">
+        <v>4285</v>
+      </c>
+      <c r="E2">
+        <v>76.470588235294102</v>
+      </c>
+      <c r="F2">
+        <v>789.74188522767099</v>
+      </c>
+      <c r="G2">
+        <v>5625</v>
+      </c>
+      <c r="I2">
+        <v>90.196078431372499</v>
+      </c>
+      <c r="J2">
+        <v>877.35462293635601</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3">
+        <v>88.235294117647001</v>
+      </c>
+      <c r="B3">
+        <v>827.75398833418899</v>
+      </c>
+      <c r="C3">
+        <v>6418</v>
+      </c>
+      <c r="E3">
+        <v>82.352941176470495</v>
+      </c>
+      <c r="F3">
+        <v>729.22501084951102</v>
+      </c>
+      <c r="G3">
+        <v>4702</v>
+      </c>
+      <c r="I3">
+        <v>94.117647058823493</v>
+      </c>
+      <c r="J3">
+        <v>814.60613142135105</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4">
+        <v>88.235294117647001</v>
+      </c>
+      <c r="B4">
+        <v>782.45089824684396</v>
+      </c>
+      <c r="C4">
+        <v>5575</v>
+      </c>
+      <c r="E4">
+        <v>82.352941176470495</v>
+      </c>
+      <c r="F4">
+        <v>792.79704890223297</v>
+      </c>
+      <c r="G4">
+        <v>5728</v>
+      </c>
+      <c r="I4">
+        <v>91.6666666666666</v>
+      </c>
+      <c r="J4">
+        <v>807.03111777933395</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5">
+        <v>86.274509803921504</v>
+      </c>
+      <c r="B5">
+        <v>764.576396249666</v>
+      </c>
+      <c r="C5">
+        <v>4186</v>
+      </c>
+      <c r="E5">
+        <v>88.235294117647001</v>
+      </c>
+      <c r="F5">
+        <v>787.42360061374404</v>
+      </c>
+      <c r="G5">
+        <v>6874</v>
+      </c>
+      <c r="I5">
+        <v>90.196078431372499</v>
+      </c>
+      <c r="J5">
+        <v>710.54901531229996</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6">
+        <v>88.235294117647001</v>
+      </c>
+      <c r="B6">
+        <v>713.37898004405395</v>
+      </c>
+      <c r="C6">
+        <v>2115</v>
+      </c>
+      <c r="E6">
+        <v>94.117647058823493</v>
+      </c>
+      <c r="F6">
+        <v>727.87881360218205</v>
+      </c>
+      <c r="G6">
+        <v>3705</v>
+      </c>
+      <c r="I6">
+        <v>84.313725490196006</v>
+      </c>
+      <c r="J6">
+        <v>786.445231139204</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7">
+        <v>88.235294117647001</v>
+      </c>
+      <c r="B7">
+        <v>721.38397425202402</v>
+      </c>
+      <c r="C7">
+        <v>2183</v>
+      </c>
+      <c r="E7">
+        <v>88.235294117647001</v>
+      </c>
+      <c r="F7">
+        <v>747.05492538114299</v>
+      </c>
+      <c r="G7">
+        <v>5613</v>
+      </c>
+      <c r="I7">
+        <v>82.352941176470495</v>
+      </c>
+      <c r="J7">
+        <v>825.45415495896498</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8">
+        <v>74.509803921568604</v>
+      </c>
+      <c r="B8">
+        <v>823.94856350048406</v>
+      </c>
+      <c r="C8">
+        <v>6471</v>
+      </c>
+      <c r="E8">
+        <v>84.313725490196006</v>
+      </c>
+      <c r="F8">
+        <v>811.24477272936394</v>
+      </c>
+      <c r="G8">
+        <v>4811</v>
+      </c>
+      <c r="I8">
+        <v>70.588235294117595</v>
+      </c>
+      <c r="J8">
+        <v>807.44002268495296</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9">
+        <v>94.117647058823493</v>
+      </c>
+      <c r="B9">
+        <v>740.35580196833098</v>
+      </c>
+      <c r="C9">
+        <v>5740</v>
+      </c>
+      <c r="E9">
+        <v>90.196078431372499</v>
+      </c>
+      <c r="F9">
+        <v>725.16240055040305</v>
+      </c>
+      <c r="G9">
+        <v>5197</v>
+      </c>
+      <c r="I9">
+        <v>82.352941176470495</v>
+      </c>
+      <c r="J9">
+        <v>729.92873630408997</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10">
+        <v>100</v>
+      </c>
+      <c r="B10">
+        <v>809.977626068007</v>
+      </c>
+      <c r="C10">
+        <v>6115</v>
+      </c>
+      <c r="E10">
+        <v>88.235294117647001</v>
+      </c>
+      <c r="F10">
+        <v>782.60799463894296</v>
+      </c>
+      <c r="G10">
+        <v>5307</v>
+      </c>
+      <c r="I10">
+        <v>82.352941176470495</v>
+      </c>
+      <c r="J10">
+        <v>867.26225287374302</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11">
+        <v>78.431372549019599</v>
+      </c>
+      <c r="B11">
+        <v>765.784224228364</v>
+      </c>
+      <c r="C11">
+        <v>3257</v>
+      </c>
+      <c r="E11">
+        <v>90.196078431372499</v>
+      </c>
+      <c r="F11">
+        <v>733.12679513401395</v>
+      </c>
+      <c r="G11">
+        <v>4238</v>
+      </c>
+      <c r="I11">
+        <v>72.549019607843107</v>
+      </c>
+      <c r="J11">
+        <v>762.56129517572003</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12">
+        <v>82.352941176470495</v>
+      </c>
+      <c r="B12">
+        <v>840.37752136845597</v>
+      </c>
+      <c r="C12">
+        <v>7259</v>
+      </c>
+      <c r="E12">
+        <v>68.627450980392098</v>
+      </c>
+      <c r="F12">
+        <v>830.77977602620899</v>
+      </c>
+      <c r="G12">
+        <v>6945</v>
+      </c>
+      <c r="I12">
+        <v>78.431372549019599</v>
+      </c>
+      <c r="J12">
+        <v>763.27319013428098</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13">
+        <v>93.478260869565204</v>
+      </c>
+      <c r="B13">
+        <v>728.294150808827</v>
+      </c>
+      <c r="C13">
+        <v>5235</v>
+      </c>
+      <c r="E13">
+        <v>85.4166666666666</v>
+      </c>
+      <c r="F13">
+        <v>728.41439474161405</v>
+      </c>
+      <c r="G13">
+        <v>4415</v>
+      </c>
+      <c r="I13">
+        <v>73.469387755102005</v>
+      </c>
+      <c r="J13">
+        <v>791.856676427053</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14">
+        <v>86.842105263157904</v>
+      </c>
+      <c r="B14">
+        <v>854.21022922608302</v>
+      </c>
+      <c r="C14">
+        <v>6284</v>
+      </c>
+      <c r="E14">
+        <v>83.870967741935402</v>
+      </c>
+      <c r="F14">
+        <v>831.31761286246001</v>
+      </c>
+      <c r="G14">
+        <v>6822</v>
+      </c>
+      <c r="I14">
+        <v>86.274509803921504</v>
+      </c>
+      <c r="J14">
+        <v>790.02455413403197</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15">
+        <v>94</v>
+      </c>
+      <c r="B15">
+        <v>585.63791689750599</v>
+      </c>
+      <c r="C15">
+        <v>1400</v>
+      </c>
+      <c r="E15">
+        <v>70.588235294117595</v>
+      </c>
+      <c r="F15">
+        <v>411.90243020893399</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>84.313725490196006</v>
+      </c>
+      <c r="J15">
+        <v>721.37567281751399</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16">
+        <v>82.352941176470495</v>
+      </c>
       <c r="B16">
-        <f>MEDIAN(A2:A11)</f>
-        <v>89.21568627450975</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19">
-      <c r="A18" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19">
-      <c r="A19" t="s">
-        <v>26</v>
-      </c>
-      <c r="E19" t="s">
-        <v>27</v>
-      </c>
-      <c r="I19" t="s">
-        <v>28</v>
-      </c>
-      <c r="M19" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19">
+        <v>697.48324257138097</v>
+      </c>
+      <c r="C16">
+        <v>554</v>
+      </c>
+      <c r="E16">
+        <v>94.117647058823493</v>
+      </c>
+      <c r="F16">
+        <v>564.08122982170005</v>
+      </c>
+      <c r="G16">
+        <v>253</v>
+      </c>
+      <c r="I16">
+        <v>90.196078431372499</v>
+      </c>
+      <c r="J16">
+        <v>727.60920311617394</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17">
+        <v>74</v>
+      </c>
+      <c r="B17">
+        <v>663.39669810094301</v>
+      </c>
+      <c r="C17">
+        <v>602</v>
+      </c>
+      <c r="E17">
+        <v>88.235294117647001</v>
+      </c>
+      <c r="F17">
+        <v>609.66911534758503</v>
+      </c>
+      <c r="G17">
+        <v>643</v>
+      </c>
+      <c r="I17">
+        <v>92.156862745097996</v>
+      </c>
+      <c r="J17">
+        <v>796.75908889060702</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18">
+        <v>84</v>
+      </c>
+      <c r="B18">
+        <v>619.77315221779395</v>
+      </c>
+      <c r="C18">
+        <v>1906</v>
+      </c>
+      <c r="E18">
+        <v>88.235294117647001</v>
+      </c>
+      <c r="F18">
+        <v>613.34396294393105</v>
+      </c>
+      <c r="G18">
+        <v>1842</v>
+      </c>
+      <c r="I18">
+        <v>84.313725490196006</v>
+      </c>
+      <c r="J18">
+        <v>757.84730375669699</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19">
+        <v>90.196078431372499</v>
+      </c>
+      <c r="B19">
+        <v>741.08743564045199</v>
+      </c>
+      <c r="C19">
+        <v>5343</v>
+      </c>
+      <c r="E19">
+        <v>92.156862745097996</v>
+      </c>
+      <c r="F19">
+        <v>776.02343905730197</v>
+      </c>
+      <c r="G19">
+        <v>5274</v>
+      </c>
+      <c r="I19">
+        <v>86.274509803921504</v>
+      </c>
+      <c r="J19">
+        <v>837.84980210929496</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
       <c r="A20">
+        <v>84.313725490196006</v>
+      </c>
+      <c r="B20">
+        <v>831.55467771832105</v>
+      </c>
+      <c r="C20">
+        <v>4345</v>
+      </c>
+      <c r="E20">
+        <v>76.470588235294102</v>
+      </c>
+      <c r="F20">
+        <v>728.844206599264</v>
+      </c>
+      <c r="G20">
+        <v>4327</v>
+      </c>
+      <c r="I20">
+        <v>92.156862745097996</v>
+      </c>
+      <c r="J20">
+        <v>789.15706657746102</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21">
+        <v>90.196078431372499</v>
+      </c>
+      <c r="B21">
+        <v>775.98925006686602</v>
+      </c>
+      <c r="C21">
+        <v>4826</v>
+      </c>
+      <c r="E21">
+        <v>62.745098039215598</v>
+      </c>
+      <c r="F21">
+        <v>829.54774481311995</v>
+      </c>
+      <c r="G21">
+        <v>6953</v>
+      </c>
+      <c r="I21">
+        <v>86.274509803921504</v>
+      </c>
+      <c r="J21">
+        <v>793.87311808053005</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23">
+        <f>MIN(A2:A21)</f>
+        <v>74</v>
+      </c>
+      <c r="E23" t="s">
+        <v>3</v>
+      </c>
+      <c r="F23">
+        <f>MIN(E2:E21)</f>
+        <v>62.745098039215598</v>
+      </c>
+      <c r="I23" t="s">
+        <v>3</v>
+      </c>
+      <c r="J23">
+        <f>MIN(I2:I21)</f>
+        <v>70.588235294117595</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24">
+        <f>MAX(A2:A21)</f>
+        <v>100</v>
+      </c>
+      <c r="E24" t="s">
+        <v>4</v>
+      </c>
+      <c r="F24">
+        <f>MAX(E2:E21)</f>
         <v>94.117647058823493</v>
       </c>
-      <c r="B20">
-        <v>770.17312879989595</v>
-      </c>
-      <c r="C20">
-        <v>4970</v>
-      </c>
-      <c r="E20">
-        <v>96.078431372549005</v>
-      </c>
-      <c r="F20">
-        <v>749.39526821672803</v>
-      </c>
-      <c r="G20">
-        <v>4638</v>
-      </c>
-      <c r="I20">
-        <v>82.352941176470495</v>
-      </c>
-      <c r="J20">
-        <v>781.66938288194103</v>
-      </c>
-      <c r="K20">
-        <v>4369</v>
-      </c>
-      <c r="M20">
-        <v>80.392156862745097</v>
-      </c>
-      <c r="N20">
-        <v>791.07893334927599</v>
-      </c>
-      <c r="O20">
-        <v>4804</v>
-      </c>
-      <c r="Q20">
-        <v>90.196078431372499</v>
-      </c>
-      <c r="R20">
-        <v>756.58171239316403</v>
-      </c>
-      <c r="S20">
-        <v>4285</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19">
-      <c r="A21">
-        <v>98.039215686274503</v>
-      </c>
-      <c r="B21">
-        <v>795.39246679357495</v>
-      </c>
-      <c r="C21">
-        <v>7077</v>
-      </c>
-      <c r="E21">
-        <v>80.392156862745097</v>
-      </c>
-      <c r="F21">
-        <v>772.19734793571104</v>
-      </c>
-      <c r="G21">
-        <v>6569</v>
-      </c>
-      <c r="I21">
-        <v>72.549019607843107</v>
-      </c>
-      <c r="J21">
-        <v>857.40650350734802</v>
-      </c>
-      <c r="K21">
-        <v>4710</v>
-      </c>
-      <c r="M21">
+      <c r="I24" t="s">
+        <v>4</v>
+      </c>
+      <c r="J24">
+        <f>MAX(I2:I21)</f>
         <v>94.117647058823493</v>
       </c>
-      <c r="N21">
-        <v>762.73930525252899</v>
-      </c>
-      <c r="O21">
-        <v>5741</v>
-      </c>
-      <c r="Q21">
-        <v>98.039215686274503</v>
-      </c>
-      <c r="R21">
-        <v>820.11334015214004</v>
-      </c>
-      <c r="S21">
-        <v>5372</v>
-      </c>
-    </row>
-    <row r="22" spans="1:19">
-      <c r="A22">
-        <v>92.156862745097996</v>
-      </c>
-      <c r="B22">
-        <v>795.37105044782504</v>
-      </c>
-      <c r="C22">
-        <v>7382</v>
-      </c>
-      <c r="E22">
-        <v>95</v>
-      </c>
-      <c r="F22">
-        <v>729.54464574009501</v>
-      </c>
-      <c r="G22">
-        <v>5075</v>
-      </c>
-      <c r="I22">
-        <v>82</v>
-      </c>
-      <c r="J22">
-        <v>784.68793293114197</v>
-      </c>
-      <c r="K22">
-        <v>6017</v>
-      </c>
-      <c r="M22">
-        <v>96.078431372549005</v>
-      </c>
-      <c r="N22">
-        <v>796.36040756301804</v>
-      </c>
-      <c r="O22">
-        <v>6301</v>
-      </c>
-      <c r="Q22">
-        <v>76</v>
-      </c>
-      <c r="R22">
-        <v>786.34411094422603</v>
-      </c>
-      <c r="S22">
-        <v>4829</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19">
-      <c r="A23">
-        <v>86.274509803921504</v>
-      </c>
-      <c r="B23">
-        <v>740.67952674033904</v>
-      </c>
-      <c r="C23">
-        <v>5088</v>
-      </c>
-      <c r="E23">
-        <v>80.392156862745097</v>
-      </c>
-      <c r="F23">
-        <v>721.51809992752601</v>
-      </c>
-      <c r="G23">
-        <v>1833</v>
-      </c>
-      <c r="I23">
-        <v>90.196078431372499</v>
-      </c>
-      <c r="J23">
-        <v>784.47282623287299</v>
-      </c>
-      <c r="K23">
-        <v>5726</v>
-      </c>
-      <c r="M23">
-        <v>82.352941176470495</v>
-      </c>
-      <c r="N23">
-        <v>774.37243739302005</v>
-      </c>
-      <c r="O23">
-        <v>5822</v>
-      </c>
-      <c r="Q23">
-        <v>94.117647058823493</v>
-      </c>
-      <c r="R23">
-        <v>719.61111819309099</v>
-      </c>
-      <c r="S23">
-        <v>8832</v>
-      </c>
-    </row>
-    <row r="24" spans="1:19">
-      <c r="A24">
-        <v>90.196078431372499</v>
-      </c>
-      <c r="B24">
-        <v>812.61298302316197</v>
-      </c>
-      <c r="C24">
-        <v>6335</v>
-      </c>
-      <c r="E24">
-        <v>86.274509803921504</v>
-      </c>
-      <c r="F24">
-        <v>728.79793710737101</v>
-      </c>
-      <c r="G24">
-        <v>2576</v>
-      </c>
-      <c r="I24">
-        <v>86.274509803921504</v>
-      </c>
-      <c r="J24">
-        <v>717.69898206713901</v>
-      </c>
-      <c r="K24">
-        <v>2415</v>
-      </c>
-      <c r="M24">
-        <v>84.313725490196006</v>
-      </c>
-      <c r="N24">
-        <v>853.60195246338503</v>
-      </c>
-      <c r="O24">
-        <v>7507</v>
-      </c>
-      <c r="Q24">
-        <v>88.235294117647001</v>
-      </c>
-      <c r="R24">
-        <v>768.62483023664402</v>
-      </c>
-      <c r="S24">
-        <v>5891</v>
-      </c>
-    </row>
-    <row r="25" spans="1:19">
-      <c r="A25">
-        <v>86.274509803921504</v>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="A25" t="s">
+        <v>33</v>
       </c>
       <c r="B25">
-        <v>748.15799519418601</v>
-      </c>
-      <c r="C25">
-        <v>6599</v>
-      </c>
-      <c r="E25">
-        <v>90.196078431372499</v>
+        <f>AVERAGE(A2:A21)</f>
+        <v>86.812096738008677</v>
+      </c>
+      <c r="E25" t="s">
+        <v>33</v>
       </c>
       <c r="F25">
-        <v>653.84359191098099</v>
-      </c>
-      <c r="G25">
-        <v>963</v>
-      </c>
-      <c r="I25">
-        <v>90.196078431372499</v>
+        <f>AVERAGE(E2:E21)</f>
+        <v>83.758499367488881</v>
+      </c>
+      <c r="I25" t="s">
+        <v>33</v>
       </c>
       <c r="J25">
-        <v>753.71662282548596</v>
-      </c>
-      <c r="K25">
-        <v>5243</v>
-      </c>
-      <c r="M25">
-        <v>90.196078431372499</v>
-      </c>
-      <c r="N25">
-        <v>770.64711124827204</v>
-      </c>
-      <c r="O25">
-        <v>5507</v>
-      </c>
-      <c r="Q25">
-        <v>90.196078431372499</v>
-      </c>
-      <c r="R25">
-        <v>844.44138264222704</v>
-      </c>
-      <c r="S25">
-        <v>5733</v>
-      </c>
-    </row>
-    <row r="26" spans="1:19">
-      <c r="A26">
-        <v>88.235294117647001</v>
+        <f>AVERAGE(I2:I21)</f>
+        <v>84.727390956382493</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="A26" t="s">
+        <v>29</v>
       </c>
       <c r="B26">
-        <v>792.39225961073396</v>
-      </c>
-      <c r="C26">
-        <v>4911</v>
-      </c>
-      <c r="E26">
-        <v>92.156862745097996</v>
+        <f>MEDIAN(A2:A21)</f>
+        <v>88.235294117647001</v>
+      </c>
+      <c r="E26" t="s">
+        <v>29</v>
       </c>
       <c r="F26">
-        <v>714.76255657235504</v>
-      </c>
-      <c r="G26">
-        <v>3214</v>
-      </c>
-      <c r="I26">
-        <v>84.313725490196006</v>
+        <f>MEDIAN(E2:E21)</f>
+        <v>86.825980392156794</v>
+      </c>
+      <c r="I26" t="s">
+        <v>29</v>
       </c>
       <c r="J26">
-        <v>832.43274089894601</v>
-      </c>
-      <c r="K26">
-        <v>6814</v>
-      </c>
-      <c r="M26">
-        <v>96.078431372549005</v>
-      </c>
-      <c r="N26">
-        <v>770.470562127074</v>
-      </c>
-      <c r="O26">
-        <v>5612</v>
-      </c>
-      <c r="Q26">
-        <v>76.470588235294102</v>
-      </c>
-      <c r="R26">
-        <v>931.16422197632903</v>
-      </c>
-      <c r="S26">
-        <v>6843</v>
-      </c>
-    </row>
-    <row r="27" spans="1:19">
-      <c r="A27">
-        <v>88.235294117647001</v>
-      </c>
-      <c r="B27">
-        <v>819.94413613193103</v>
-      </c>
-      <c r="C27">
-        <v>5068</v>
-      </c>
-      <c r="E27">
-        <v>86.274509803921504</v>
-      </c>
-      <c r="F27">
-        <v>781.74246210550598</v>
-      </c>
-      <c r="G27">
-        <v>5765</v>
-      </c>
-      <c r="I27">
-        <v>86.274509803921504</v>
-      </c>
-      <c r="J27">
-        <v>831.833241900453</v>
-      </c>
-      <c r="K27">
-        <v>5405</v>
-      </c>
-      <c r="M27">
-        <v>88.235294117647001</v>
-      </c>
-      <c r="N27">
-        <v>733.24608544498199</v>
-      </c>
-      <c r="O27">
-        <v>5924</v>
-      </c>
-      <c r="Q27">
-        <v>88.235294117647001</v>
-      </c>
-      <c r="R27">
-        <v>874.41508906403101</v>
-      </c>
-      <c r="S27">
-        <v>5387</v>
-      </c>
-    </row>
-    <row r="28" spans="1:19">
-      <c r="A28">
-        <v>82.352941176470495</v>
-      </c>
-      <c r="B28">
-        <v>783.27148625442101</v>
-      </c>
-      <c r="C28">
-        <v>6628</v>
-      </c>
-      <c r="E28">
-        <v>94.117647058823493</v>
-      </c>
-      <c r="F28">
-        <v>827.25439537822297</v>
-      </c>
-      <c r="G28">
-        <v>5775</v>
-      </c>
-      <c r="I28">
-        <v>90.196078431372499</v>
-      </c>
-      <c r="J28">
-        <v>818.84339887792805</v>
-      </c>
-      <c r="K28">
-        <v>5773</v>
-      </c>
-      <c r="M28">
-        <v>88.235294117647001</v>
-      </c>
-      <c r="N28">
-        <v>739.37913831708397</v>
-      </c>
-      <c r="O28">
-        <v>3545</v>
-      </c>
-      <c r="Q28">
-        <v>90.196078431372499</v>
-      </c>
-      <c r="R28">
-        <v>847.00532203181899</v>
-      </c>
-      <c r="S28">
-        <v>6260</v>
-      </c>
-    </row>
-    <row r="29" spans="1:19">
-      <c r="A29">
-        <v>82.352941176470495</v>
-      </c>
-      <c r="B29">
-        <v>843.02185636310401</v>
-      </c>
-      <c r="C29">
-        <v>4813</v>
-      </c>
-      <c r="E29">
-        <v>84.313725490196006</v>
-      </c>
-      <c r="F29">
-        <v>809.83399915048301</v>
-      </c>
-      <c r="G29">
-        <v>4866</v>
-      </c>
-      <c r="I29">
-        <v>76.470588235294102</v>
-      </c>
-      <c r="J29">
-        <v>776.99092006283797</v>
-      </c>
-      <c r="K29">
-        <v>4535</v>
-      </c>
-      <c r="M29">
-        <v>90.196078431372499</v>
-      </c>
-      <c r="N29">
-        <v>760.90801855924406</v>
-      </c>
-      <c r="O29">
-        <v>6263</v>
-      </c>
-      <c r="Q29">
-        <v>94.117647058823493</v>
-      </c>
-      <c r="R29">
-        <v>830.35268415934104</v>
-      </c>
-      <c r="S29">
-        <v>5005</v>
-      </c>
-    </row>
-    <row r="30" spans="1:19">
-      <c r="Q30">
-        <v>90.196078431372499</v>
-      </c>
-      <c r="R30">
-        <v>787.70666282135801</v>
-      </c>
-      <c r="S30">
-        <v>13257</v>
-      </c>
-    </row>
-    <row r="31" spans="1:19">
-      <c r="A31" t="s">
-        <v>3</v>
-      </c>
-      <c r="B31">
-        <f>MIN(A20:A29)</f>
-        <v>82.352941176470495</v>
-      </c>
-      <c r="E31" t="s">
-        <v>3</v>
-      </c>
-      <c r="F31">
-        <f>MIN(E20:E29)</f>
-        <v>80.392156862745097</v>
-      </c>
-      <c r="I31" t="s">
-        <v>3</v>
-      </c>
-      <c r="J31">
-        <f>MIN(I20:I29)</f>
-        <v>72.549019607843107</v>
-      </c>
-      <c r="M31" t="s">
-        <v>3</v>
-      </c>
-      <c r="N31">
-        <f>MIN(M20:M29)</f>
-        <v>80.392156862745097</v>
-      </c>
-      <c r="Q31">
-        <v>74.509803921568604</v>
-      </c>
-      <c r="R31">
-        <v>892.39361398721906</v>
-      </c>
-      <c r="S31">
-        <v>5273</v>
-      </c>
-    </row>
-    <row r="32" spans="1:19">
-      <c r="A32" t="s">
-        <v>4</v>
-      </c>
-      <c r="B32">
-        <f>MAX(A20:A29)</f>
-        <v>98.039215686274503</v>
-      </c>
-      <c r="E32" t="s">
-        <v>4</v>
-      </c>
-      <c r="F32">
-        <f>MAX(E20:E29)</f>
-        <v>96.078431372549005</v>
-      </c>
-      <c r="I32" t="s">
-        <v>4</v>
-      </c>
-      <c r="J32">
-        <f>MAX(I20:I29)</f>
-        <v>90.196078431372499</v>
-      </c>
-      <c r="M32" t="s">
-        <v>4</v>
-      </c>
-      <c r="N32">
-        <f>MAX(M20:M29)</f>
-        <v>96.078431372549005</v>
-      </c>
-      <c r="Q32">
-        <v>90.196078431372499</v>
-      </c>
-      <c r="R32">
-        <v>808.38680182663097</v>
-      </c>
-      <c r="S32">
-        <v>11731</v>
-      </c>
-    </row>
-    <row r="33" spans="1:19">
-      <c r="A33" t="s">
-        <v>5</v>
-      </c>
-      <c r="B33">
-        <f>AVERAGE(A20:A29)</f>
-        <v>88.823529411764639</v>
-      </c>
-      <c r="E33" t="s">
-        <v>5</v>
-      </c>
-      <c r="F33">
-        <f>AVERAGE(E20:E29)</f>
-        <v>88.519607843137223</v>
-      </c>
-      <c r="I33" t="s">
-        <v>5</v>
-      </c>
-      <c r="J33">
-        <f>AVERAGE(I20:I29)</f>
-        <v>84.082352941176424</v>
-      </c>
-      <c r="M33" t="s">
-        <v>5</v>
-      </c>
-      <c r="N33">
-        <f>AVERAGE(M20:M29)</f>
-        <v>89.019607843137209</v>
-      </c>
-      <c r="Q33">
-        <v>94.117647058823493</v>
-      </c>
-      <c r="R33">
-        <v>729.85457422329102</v>
-      </c>
-      <c r="S33">
-        <v>4206</v>
-      </c>
-    </row>
-    <row r="34" spans="1:19">
-      <c r="Q34">
-        <v>84.313725490196006</v>
-      </c>
-      <c r="R34">
-        <v>843.03460671236803</v>
-      </c>
-      <c r="S34">
-        <v>5834</v>
-      </c>
-    </row>
-    <row r="35" spans="1:19">
-      <c r="Q35">
-        <v>88.235294117647001</v>
-      </c>
-      <c r="R35">
-        <v>826.287500786279</v>
-      </c>
-      <c r="S35">
-        <v>6844</v>
-      </c>
-    </row>
-    <row r="36" spans="1:19">
-      <c r="Q36">
-        <v>94.117647058823493</v>
-      </c>
-      <c r="R36">
-        <v>790.47650635060495</v>
-      </c>
-      <c r="S36">
-        <v>5266</v>
-      </c>
-    </row>
-    <row r="37" spans="1:19">
-      <c r="Q37">
-        <v>86.274509803921504</v>
-      </c>
-      <c r="R37">
-        <v>753.14397739178503</v>
-      </c>
-      <c r="S37">
-        <v>3814</v>
-      </c>
-    </row>
-    <row r="38" spans="1:19">
-      <c r="Q38">
-        <v>96.078431372549005</v>
-      </c>
-      <c r="R38">
-        <v>788.72538952217803</v>
-      </c>
-      <c r="S38">
-        <v>5433</v>
-      </c>
-    </row>
-    <row r="39" spans="1:19">
-      <c r="Q39">
-        <v>90.196078431372499</v>
-      </c>
-      <c r="R39">
-        <v>809.09418052815499</v>
-      </c>
-      <c r="S39">
-        <v>5957</v>
-      </c>
-    </row>
-    <row r="41" spans="1:19">
-      <c r="R41">
-        <f>MIN(Q20:Q39)</f>
-        <v>74.509803921568604</v>
-      </c>
-    </row>
-    <row r="42" spans="1:19">
-      <c r="R42">
-        <f>MAX(Q20:Q39)</f>
-        <v>98.039215686274503</v>
-      </c>
-    </row>
-    <row r="43" spans="1:19">
-      <c r="R43">
-        <f>AVERAGE(Q20:Q39)</f>
-        <v>88.701960784313684</v>
-      </c>
-    </row>
-    <row r="44" spans="1:19">
-      <c r="Q44" t="s">
-        <v>29</v>
-      </c>
-      <c r="R44">
-        <f>MEDIAN(Q20:Q39)</f>
-        <v>90.196078431372499</v>
+        <f>MEDIAN(I2:I21)</f>
+        <v>85.294117647058755</v>
       </c>
     </row>
   </sheetData>

</xml_diff>